<commit_message>
update BOM D2 D3 D4
</commit_message>
<xml_diff>
--- a/BOM/BOM_Driver Board _2025-07-23.xlsx
+++ b/BOM/BOM_Driver Board _2025-07-23.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6400B2F1-C76E-4FD1-A25E-1137A1C210C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="BOM_Driver Board V3.0_Schematic" state="visible" r:id="rId4"/>
+    <sheet name="BOM_Driver Board V3.0_Schematic" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="199">
   <si>
     <t>No.</t>
   </si>
@@ -178,12 +182,6 @@
     <t>SMA_L4.3-W2.6-LS5.0-FD</t>
   </si>
   <si>
-    <t>D2,D3,D4</t>
-  </si>
-  <si>
-    <t>C7420365,C7420367</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -193,422 +191,454 @@
     <t>SOD-523_L1.2-W0.8-LS1.6-FD</t>
   </si>
   <si>
+    <t>C19077463</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>FXL0420-100-M</t>
+  </si>
+  <si>
+    <t>cjiang(长江微电)</t>
+  </si>
+  <si>
+    <t>10uH ±20% 2.2A</t>
+  </si>
+  <si>
+    <t>IND-SMD_L4.4-W4.2</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>C177242</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>FXL0630-4R7-M</t>
+  </si>
+  <si>
+    <t>4.7uH ±20% 9A</t>
+  </si>
+  <si>
+    <t>IND-SMD_L7.0-W6.6</t>
+  </si>
+  <si>
+    <t>4.7uH</t>
+  </si>
+  <si>
+    <t>L2,L3</t>
+  </si>
+  <si>
+    <t>C167220</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>2.54mm</t>
+  </si>
+  <si>
+    <t>卧贴排母 2.54mm 4P</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>0603WAJ0102T5E</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(厚声)</t>
+  </si>
+  <si>
+    <t>1kΩ ±5% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>1kΩ</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>C25585</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>0603WAJ0103T5E</t>
+  </si>
+  <si>
+    <t>10kΩ ±5% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>R2,R5,R9,R10,R18</t>
+  </si>
+  <si>
+    <t>C15401</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>FRC0603F1302TS</t>
+  </si>
+  <si>
+    <t>电阻</t>
+  </si>
+  <si>
+    <t>贴片电阻</t>
+  </si>
+  <si>
+    <t>FOJAN(富捷)</t>
+  </si>
+  <si>
+    <t>13kΩ ±1% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>13kΩ</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>C2906992</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>FRC0603F4301TS</t>
+  </si>
+  <si>
+    <t>4.3kΩ ±1% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>4.3kΩ</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C2930099</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>0603WAF2003T5E</t>
+  </si>
+  <si>
+    <t>200kΩ ±1% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>200kΩ</t>
+  </si>
+  <si>
+    <t>R6,R13</t>
+  </si>
+  <si>
+    <t>C25811</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>1206W4F500LT5E</t>
+  </si>
+  <si>
+    <t>500mΩ ±1% 250mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>500mΩ</t>
+  </si>
+  <si>
+    <t>R7,R14</t>
+  </si>
+  <si>
+    <t>C25340</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>厚膜电阻 4.7kΩ ±1% 100mW</t>
+  </si>
+  <si>
+    <t>4.7kΩ</t>
+  </si>
+  <si>
+    <t>R8,R15</t>
+  </si>
+  <si>
+    <t>C99782</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>0603WAF9101T5E</t>
+  </si>
+  <si>
+    <t>9.1kΩ ±1% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>9.1kΩ</t>
+  </si>
+  <si>
+    <t>R11,R12</t>
+  </si>
+  <si>
+    <t>C23260</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>0603WAF5100T5E</t>
+  </si>
+  <si>
+    <t>510Ω ±1% 100mW 厚膜电阻</t>
+  </si>
+  <si>
+    <t>510Ω</t>
+  </si>
+  <si>
+    <t>R16,R17</t>
+  </si>
+  <si>
+    <t>C23193</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>M2螺丝</t>
+  </si>
+  <si>
+    <t>SCREW1,SCREW2</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>CH224K</t>
+  </si>
+  <si>
+    <t>通信接口芯片/UART/485/232</t>
+  </si>
+  <si>
+    <t>USB芯片</t>
+  </si>
+  <si>
+    <t>WCH(南京沁恒)</t>
+  </si>
+  <si>
+    <t>USB PD等多快充协议受电芯片CH224</t>
+  </si>
+  <si>
+    <t>ESSOP-10_L4.9-W3.9-P1.0-LS6.0-TL-EP</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>C970725</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>LGS5145</t>
+  </si>
+  <si>
+    <t>电源管理</t>
+  </si>
+  <si>
+    <t>DC-DC电源芯片</t>
+  </si>
+  <si>
+    <t>Legend-Si(棱晶半导体)</t>
+  </si>
+  <si>
+    <t>高效率异步降压转换器</t>
+  </si>
+  <si>
+    <t>SOT-23-6_L2.9-W1.7-P0.95-LS2.8-BL</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C5123971</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>ESP8684-MINI-1U-H4</t>
+  </si>
+  <si>
+    <t>物联网/通信模块</t>
+  </si>
+  <si>
+    <t>蓝牙模块</t>
+  </si>
+  <si>
+    <t>ESPRESSIF(乐鑫)</t>
+  </si>
+  <si>
+    <t>WIFIM-SMD_61P-L13.2-W12.5-P0.80</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>C7497295</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>LGS63042EP</t>
+  </si>
+  <si>
+    <t>数码管驱动/LED驱动</t>
+  </si>
+  <si>
+    <t>LED驱动</t>
+  </si>
+  <si>
+    <t>输出1.2A PWM调光 降压,升压型驱动</t>
+  </si>
+  <si>
+    <t>ESOP-8_L4.9-W3.9-P1.27-LS6.0-TL-EP3.3</t>
+  </si>
+  <si>
+    <t>U4,U5</t>
+  </si>
+  <si>
+    <t>C5280696</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>ZX-MX1.25-4PWT</t>
+  </si>
+  <si>
+    <t>连接器</t>
+  </si>
+  <si>
+    <t>线对板针座</t>
+  </si>
+  <si>
+    <t>Megastar(兆星)</t>
+  </si>
+  <si>
+    <t>1x4P 间距:1.25mm 卧贴 系列:PicoBlade(MX 1.25) 配套胶壳型号：ZX-MX1.25-4PJK 配套端子型号：ZX-MX1.25-DZ 配套杜邦线型号：ZX-MX1.25-4PBXC</t>
+  </si>
+  <si>
+    <t>CONN-SMD_4P-P1.25-MX1.25-4P-WT</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>C7430470</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>TYPE-C 6P(073)</t>
+  </si>
+  <si>
+    <t>SHOU HAN(首韩)</t>
+  </si>
+  <si>
+    <t>Type-C 母 卧贴</t>
+  </si>
+  <si>
+    <t>TYPE-C-SMD_TYPE-C-6P-073</t>
+  </si>
+  <si>
+    <t>USB1</t>
+  </si>
+  <si>
+    <t>C668623</t>
+  </si>
+  <si>
+    <t>SS34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电压:60V 电流:3A,电压:60V 电流:3A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>D5,D6</t>
-  </si>
-  <si>
-    <t>C19077463</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>FXL0420-100-M</t>
-  </si>
-  <si>
-    <t>cjiang(长江微电)</t>
-  </si>
-  <si>
-    <t>10uH ±20% 2.2A</t>
-  </si>
-  <si>
-    <t>IND-SMD_L4.4-W4.2</t>
-  </si>
-  <si>
-    <t>10uH</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>C177242</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>FXL0630-4R7-M</t>
-  </si>
-  <si>
-    <t>4.7uH ±20% 9A</t>
-  </si>
-  <si>
-    <t>IND-SMD_L7.0-W6.6</t>
-  </si>
-  <si>
-    <t>4.7uH</t>
-  </si>
-  <si>
-    <t>L2,L3</t>
-  </si>
-  <si>
-    <t>C167220</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>2.54mm</t>
-  </si>
-  <si>
-    <t>卧贴排母 2.54mm 4P</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>0603WAJ0102T5E</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(厚声)</t>
-  </si>
-  <si>
-    <t>1kΩ ±5% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>1kΩ</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>C25585</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>0603WAJ0103T5E</t>
-  </si>
-  <si>
-    <t>10kΩ ±5% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
-    <t>R2,R5,R9,R10,R18</t>
-  </si>
-  <si>
-    <t>C15401</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>FRC0603F1302TS</t>
-  </si>
-  <si>
-    <t>电阻</t>
-  </si>
-  <si>
-    <t>贴片电阻</t>
-  </si>
-  <si>
-    <t>FOJAN(富捷)</t>
-  </si>
-  <si>
-    <t>13kΩ ±1% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>13kΩ</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>C2906992</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>FRC0603F4301TS</t>
-  </si>
-  <si>
-    <t>4.3kΩ ±1% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>4.3kΩ</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>C2930099</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>0603WAF2003T5E</t>
-  </si>
-  <si>
-    <t>200kΩ ±1% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>200kΩ</t>
-  </si>
-  <si>
-    <t>R6,R13</t>
-  </si>
-  <si>
-    <t>C25811</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>1206W4F500LT5E</t>
-  </si>
-  <si>
-    <t>500mΩ ±1% 250mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>R1206</t>
-  </si>
-  <si>
-    <t>500mΩ</t>
-  </si>
-  <si>
-    <t>R7,R14</t>
-  </si>
-  <si>
-    <t>C25340</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>RC0603FR-074K7L</t>
-  </si>
-  <si>
-    <t>厚膜电阻 4.7kΩ ±1% 100mW</t>
-  </si>
-  <si>
-    <t>4.7kΩ</t>
-  </si>
-  <si>
-    <t>R8,R15</t>
-  </si>
-  <si>
-    <t>C99782</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>0603WAF9101T5E</t>
-  </si>
-  <si>
-    <t>9.1kΩ ±1% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>9.1kΩ</t>
-  </si>
-  <si>
-    <t>R11,R12</t>
-  </si>
-  <si>
-    <t>C23260</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>0603WAF5100T5E</t>
-  </si>
-  <si>
-    <t>510Ω ±1% 100mW 厚膜电阻</t>
-  </si>
-  <si>
-    <t>510Ω</t>
-  </si>
-  <si>
-    <t>R16,R17</t>
-  </si>
-  <si>
-    <t>C23193</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>M2螺丝</t>
-  </si>
-  <si>
-    <t>SCREW1,SCREW2</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>CH224K</t>
-  </si>
-  <si>
-    <t>通信接口芯片/UART/485/232</t>
-  </si>
-  <si>
-    <t>USB芯片</t>
-  </si>
-  <si>
-    <t>WCH(南京沁恒)</t>
-  </si>
-  <si>
-    <t>USB PD等多快充协议受电芯片CH224</t>
-  </si>
-  <si>
-    <t>ESSOP-10_L4.9-W3.9-P1.0-LS6.0-TL-EP</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>C970725</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>LGS5145</t>
-  </si>
-  <si>
-    <t>电源管理</t>
-  </si>
-  <si>
-    <t>DC-DC电源芯片</t>
-  </si>
-  <si>
-    <t>Legend-Si(棱晶半导体)</t>
-  </si>
-  <si>
-    <t>高效率异步降压转换器</t>
-  </si>
-  <si>
-    <t>SOT-23-6_L2.9-W1.7-P0.95-LS2.8-BL</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>C5123971</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>ESP8684-MINI-1U-H4</t>
-  </si>
-  <si>
-    <t>物联网/通信模块</t>
-  </si>
-  <si>
-    <t>蓝牙模块</t>
-  </si>
-  <si>
-    <t>ESPRESSIF(乐鑫)</t>
-  </si>
-  <si>
-    <t>WIFIM-SMD_61P-L13.2-W12.5-P0.80</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>C7497295</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>LGS63042EP</t>
-  </si>
-  <si>
-    <t>数码管驱动/LED驱动</t>
-  </si>
-  <si>
-    <t>LED驱动</t>
-  </si>
-  <si>
-    <t>输出1.2A PWM调光 降压,升压型驱动</t>
-  </si>
-  <si>
-    <t>ESOP-8_L4.9-W3.9-P1.27-LS6.0-TL-EP3.3</t>
-  </si>
-  <si>
-    <t>U4,U5</t>
-  </si>
-  <si>
-    <t>C5280696</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>ZX-MX1.25-4PWT</t>
-  </si>
-  <si>
-    <t>连接器</t>
-  </si>
-  <si>
-    <t>线对板针座</t>
-  </si>
-  <si>
-    <t>Megastar(兆星)</t>
-  </si>
-  <si>
-    <t>1x4P 间距:1.25mm 卧贴 系列:PicoBlade(MX 1.25) 配套胶壳型号：ZX-MX1.25-4PJK 配套端子型号：ZX-MX1.25-DZ 配套杜邦线型号：ZX-MX1.25-4PBXC</t>
-  </si>
-  <si>
-    <t>CONN-SMD_4P-P1.25-MX1.25-4P-WT</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>C7430470</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>TYPE-C 6P(073)</t>
-  </si>
-  <si>
-    <t>SHOU HAN(首韩)</t>
-  </si>
-  <si>
-    <t>Type-C 母 卧贴</t>
-  </si>
-  <si>
-    <t>TYPE-C-SMD_TYPE-C-6P-073</t>
-  </si>
-  <si>
-    <t>USB1</t>
-  </si>
-  <si>
-    <t>C668623</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3,D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C7420365</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C7420367</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -635,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -971,12 +1001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
@@ -1196,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -1217,56 +1249,56 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>194</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1275,33 +1307,33 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1310,103 +1342,103 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
         <v>64</v>
       </c>
-      <c r="F10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" t="s">
-        <v>74</v>
-      </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1415,138 +1447,138 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
         <v>84</v>
       </c>
-      <c r="F13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
         <v>86</v>
-      </c>
-      <c r="H13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" t="s">
         <v>98</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s">
         <v>99</v>
       </c>
-      <c r="E15" t="s">
+      <c r="I15" t="s">
         <v>100</v>
-      </c>
-      <c r="F15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
-        <v>109</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1555,33 +1587,33 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="I17" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="J17">
         <v>2</v>
       </c>
       <c r="K17" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -1590,33 +1622,33 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I18" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="J18">
         <v>2</v>
       </c>
       <c r="K18" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -1625,33 +1657,33 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="J19">
         <v>2</v>
       </c>
       <c r="K19" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -1660,33 +1692,33 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
       <c r="K20" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -1695,245 +1727,281 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="I21" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
       <c r="K21" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>150</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H22" t="s">
         <v>13</v>
       </c>
       <c r="I22" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="G23" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="H23" t="s">
         <v>13</v>
       </c>
       <c r="I23" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="H24" t="s">
         <v>13</v>
       </c>
       <c r="I24" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E25" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F25" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H25" t="s">
         <v>13</v>
       </c>
       <c r="I25" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="F26" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G26" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H26" t="s">
         <v>13</v>
       </c>
       <c r="I26" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F27" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="G27" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="H27" t="s">
         <v>13</v>
       </c>
       <c r="I27" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>187</v>
+      </c>
+      <c r="F28" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" t="s">
+        <v>189</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>